<commit_message>
Resolution page for Pocket 6K.
</commit_message>
<xml_diff>
--- a/src/Supporting Documents/Camera Res Codec FPS Tables.xlsx
+++ b/src/Supporting Documents/Camera Res Codec FPS Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\T-Display-S3\Magic Pocket Control ESP32 PlatformIO\Magic Pocket Control ESP32\src\Supporting Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2188BFFA-C829-432D-81AF-E112D3678192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D642BB53-8F72-4C50-BFE8-C7DEC4606F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22944" yWindow="0" windowWidth="23232" windowHeight="25296" xr2:uid="{CF423722-2C23-467D-BC4A-0175CDE58A17}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="34560" windowHeight="18600" xr2:uid="{CF423722-2C23-467D-BC4A-0175CDE58A17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t>Codec</t>
   </si>
@@ -494,9 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA07B453-18D6-48FE-B90D-DB042716337C}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Pocket 4K Resolution screen
</commit_message>
<xml_diff>
--- a/src/Supporting Documents/Camera Res Codec FPS Tables.xlsx
+++ b/src/Supporting Documents/Camera Res Codec FPS Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\T-Display-S3\Magic Pocket Control ESP32 PlatformIO\Magic Pocket Control ESP32\src\Supporting Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D642BB53-8F72-4C50-BFE8-C7DEC4606F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14272CA0-B31C-4481-B437-D0977E11315A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="34560" windowHeight="18600" xr2:uid="{CF423722-2C23-467D-BC4A-0175CDE58A17}"/>
+    <workbookView xWindow="27924" yWindow="12600" windowWidth="18252" windowHeight="12696" xr2:uid="{CF423722-2C23-467D-BC4A-0175CDE58A17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA07B453-18D6-48FE-B90D-DB042716337C}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -838,7 +840,7 @@
         <v>2880</v>
       </c>
       <c r="D27">
-        <v>2116</v>
+        <v>2160</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>

</xml_diff>